<commit_message>
Fix paths for executable
</commit_message>
<xml_diff>
--- a/SampleTeam copy 2/SampleTeam3.xlsx
+++ b/SampleTeam copy 2/SampleTeam3.xlsx
@@ -461,12 +461,12 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>Contribution of research to your skill/knowledge</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>Your Full Name</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Contribution of research to your skill/knowledge</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
@@ -536,54 +536,54 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ACYDBNgFmCKENuYPaUK7PwQEYn3Qmf-KB11FTLmY06pho_S5O31EvbnJeGcVddansKof_xQ</t>
+          <t>ACYDBNij8LvaSXSmxv95us-eta_A0kXubeGiWImyFqPE3bTxeD0yzWbNFu1to7AInMRLR2M</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2024-11-01T22:05:45.716Z</t>
+          <t>2024-11-02T01:50:20.749Z</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2024-11-01T22:05:45.716673Z</t>
+          <t>2024-11-02T01:50:20.749270Z</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
           <t>6</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
       <c r="G2" t="inlineStr">
         <is>
+          <t>Satisfactory</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
           <t>asdf</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
         <is>
           <t>Satisfactory</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>Satisfactory</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>Satisfactory</t>
-        </is>
-      </c>
       <c r="L2" t="inlineStr">
         <is>
           <t>asdf</t>
@@ -596,12 +596,12 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>8</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>asdf</t>
+          <t>ads</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">

</xml_diff>